<commit_message>
updated unh_id to unique and updated views
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t xml:space="preserve">Last Name</t>
   </si>
@@ -302,23 +299,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="35.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="35.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -399,28 +396,28 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>6172072977</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>6172072977</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>33</v>
@@ -428,17 +425,17 @@
       <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>2015</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>37</v>
@@ -446,60 +443,60 @@
       <c r="O2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="3"/>
       <c r="U2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="1" t="n">
+        <v>3101</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="1" t="n">
-        <v>3101</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="B3" s="0" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="0" t="n">
+        <v>6172072977</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>6172072977</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>33</v>
@@ -507,17 +504,17 @@
       <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>2015</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>37</v>
@@ -525,46 +522,43 @@
       <c r="O3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="3"/>
       <c r="U3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="1" t="n">
+        <v>3101</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="1" t="n">
-        <v>3101</v>
-      </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="4" t="s">
+      <c r="AA3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AA2" r:id="rId1" display="Matt.baillargeon@SSBbartgroup.com"/>
-    <hyperlink ref="AA3" r:id="rId2" display="Matt.baillargeon@SSBbartgroup.com"/>
+    <hyperlink ref="Z2" r:id="rId1" display="Matt.baillargeon@SSBbartgroup.com"/>
+    <hyperlink ref="Z3" r:id="rId2" display="Matt.baillargeon@SSBbartgroup.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>